<commit_message>
reorganizing Cli project implementing DataImporter
</commit_message>
<xml_diff>
--- a/ApplicationTracker.ImportCli/Assets/sample_data.xlsx
+++ b/ApplicationTracker.ImportCli/Assets/sample_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\github\ApplicationTracker\ApplicationTracker.ImportCli\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A3EBA0-44E3-4472-A2C0-A6DC33683329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46AFDC5A-E448-4261-9D5A-82DE09559741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="23385" windowHeight="12075" xr2:uid="{85E2FF32-29DA-4025-9424-E1DA14A398A2}"/>
+    <workbookView xWindow="14655" yWindow="855" windowWidth="23385" windowHeight="12075" xr2:uid="{85E2FF32-29DA-4025-9424-E1DA14A398A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -189,6 +190,12 @@
   </si>
   <si>
     <t>Backend .NET Developer</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>Redmond</t>
   </si>
 </sst>
 </file>
@@ -246,19 +253,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -605,7 +610,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,460 +659,396 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>45475</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>45475</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>45475</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>45475</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>45487</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <v>45487</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>45487</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="4"/>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>45487</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="4"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>45490</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="4"/>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="1">
         <v>45490</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="1">
         <v>45490</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="1">
         <v>45490</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="6">
         <v>45491</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="4"/>
+      <c r="E14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="1">
         <v>45491</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="1">
         <v>45493</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="1">
         <v>45494</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="1">
         <v>45495</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="1">
         <v>45495</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="1">
         <v>45495</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="1">
         <v>45495</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>

</xml_diff>